<commit_message>
Removed 'Fvd - Almelo' from the input (Coordinates.xlsx) and from the results (including validation output). This is done due to consistency. This should not affect the functionality of the program and it does not affect any other files or results.
</commit_message>
<xml_diff>
--- a/Experiment/Input/Coordinates.xlsx
+++ b/Experiment/Input/Coordinates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdare\PycharmProjects\Information-Retrieval---Selenium\Experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdare\PycharmProjects\Information-Retrieval---Selenium\Experiment\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71C768D-A334-4339-883E-042E3B67B9AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B14086-B02C-4BF2-AF83-F4AFFB36AEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="593" xr2:uid="{2E2B948F-80FD-41A8-A50B-9CAD7A901E77}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="593" activeTab="3" xr2:uid="{2E2B948F-80FD-41A8-A50B-9CAD7A901E77}"/>
   </bookViews>
   <sheets>
     <sheet name="PVV" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
   <si>
     <t>{"latitude": 52.3545828, "longitude": 4.7638762, "accuracy": 1}</t>
   </si>
@@ -173,12 +173,6 @@
     <t>24.0</t>
   </si>
   <si>
-    <t>Almelo</t>
-  </si>
-  <si>
-    <t>16.0</t>
-  </si>
-  <si>
     <t>27.8</t>
   </si>
   <si>
@@ -228,9 +222,6 @@
   </si>
   <si>
     <t>{"latitude": 52.3810687, "longitude": 4.5187475, "accuracy": 1}</t>
-  </si>
-  <si>
-    <t>{"latitude": 52.3609531, "longitude": 6.5892449, "accuracy": 1}</t>
   </si>
   <si>
     <t>{"latitude": 52.4091256, "longitude": 6.7430093, "accuracy": 1}</t>
@@ -653,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC47F84F-EE69-4616-9EC2-9CB761F80028}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -696,7 +687,7 @@
         <v>4.5062265000000004</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -715,7 +706,7 @@
         <v>5.9724237999999996</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -779,7 +770,7 @@
         <v>5.5121256000000001</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -798,7 +789,7 @@
         <v>4.1637452000000001</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -817,7 +808,7 @@
         <v>6.1214943000000002</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -836,7 +827,7 @@
         <v>6.3700716999999996</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -898,7 +889,7 @@
         <v>6.7430092999999998</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -917,7 +908,7 @@
         <v>5.6560836999999999</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -936,7 +927,7 @@
         <v>6.1964119000000002</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -955,7 +946,7 @@
         <v>5.2373018</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -990,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{560078F0-0554-4AC1-907E-349181259D29}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1033,7 +1024,7 @@
         <v>5.0403517999999998</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1050,7 +1041,7 @@
         <v>4.0557648999999998</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1067,7 +1058,7 @@
         <v>4.1485715000000001</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1084,25 +1075,11 @@
         <v>4.5187474999999999</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6">
-        <v>52.360953100000003</v>
-      </c>
-      <c r="D6">
-        <v>6.5892448999999997</v>
-      </c>
-      <c r="E6" t="s">
-        <v>63</v>
-      </c>
+      <c r="C6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1149,7 +1126,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="10">
         <v>52.084166000000003</v>
@@ -1158,7 +1135,7 @@
         <v>5.0124515000000001</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1166,7 +1143,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" s="9">
         <v>52.354582800000003</v>
@@ -1183,7 +1160,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" s="9">
         <v>51.842841300000003</v>
@@ -1192,7 +1169,7 @@
         <v>5.7631167000000003</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1200,7 +1177,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="9">
         <v>53.221684500000002</v>
@@ -1209,7 +1186,7 @@
         <v>6.4956534000000001</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1256,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7">
         <v>52.242501900000001</v>
@@ -1274,7 +1251,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4">
         <v>52.141033399999998</v>
@@ -1283,7 +1260,7 @@
         <v>4.3034182000000003</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -1292,7 +1269,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" s="3">
         <v>52.415114199999998</v>
@@ -1301,7 +1278,7 @@
         <v>4.5523354999999999</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -1319,7 +1296,7 @@
         <v>4.6242571000000003</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3"/>
     </row>

</xml_diff>